<commit_message>
finishing but still use xlwings and streamlit qrcode scanner
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bekerja\Portfolio\qrcode-presence-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67638CD-0786-4A89-A889-29C2BFCDE589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FE4349-8B4B-4D6A-96D6-97058DB3DF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13470" yWindow="1275" windowWidth="9360" windowHeight="7965" xr2:uid="{4B390959-5403-42AF-8FD9-84DBA51F3BE3}"/>
+    <workbookView xWindow="14445" yWindow="0" windowWidth="6045" windowHeight="11040" xr2:uid="{4B390959-5403-42AF-8FD9-84DBA51F3BE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>aku</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>HADIR</t>
-  </si>
-  <si>
-    <t>anumuhafidz</t>
   </si>
 </sst>
 </file>
@@ -412,10 +409,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BE525AB-7991-4C3E-B4A3-664167BD5F02}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,13 +448,23 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45083.294571759259</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45083.298587962963</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -468,12 +475,6 @@
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
-      </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>